<commit_message>
Re-publish with correction on Extension Address Key
</commit_message>
<xml_diff>
--- a/docs/Extension-UKCore-AddressKey.xlsx
+++ b/docs/Extension-UKCore-AddressKey.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AJ$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AJ$24</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="90">
   <si>
     <t>Path</t>
   </si>
@@ -151,9 +151,6 @@
 ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Extension.id</t>
   </si>
   <si>
@@ -179,64 +176,103 @@
     <t>Extension.extension</t>
   </si>
   <si>
+    <t xml:space="preserve">Extension
+</t>
+  </si>
+  <si>
+    <t>An Extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Address Key Type</t>
+  </si>
+  <si>
+    <t>To identify the type of Address Key recorded.</t>
+  </si>
+  <si>
+    <t>Extension.extension.id</t>
+  </si>
+  <si>
+    <t>Extension.extension.extension</t>
+  </si>
+  <si>
     <t>extensions
 user content</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension
+    <t>Additional content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+  </si>
+  <si>
+    <t>Extension.extension.extension.id</t>
+  </si>
+  <si>
+    <t>Extension.extension.extension.extension</t>
+  </si>
+  <si>
+    <t>Extension.extension.extension.url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uri
 </t>
   </si>
   <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:url}
+    <t>identifies the meaning of the extension</t>
+  </si>
+  <si>
+    <t>Source of the definition for the extension code - a logical name or a URL.</t>
+  </si>
+  <si>
+    <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
+  </si>
+  <si>
+    <t>Extension.url</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Extension.extension.extension.value[x]</t>
+  </si>
+  <si>
+    <t>base64Binary
+booleancanonicalcodedatedateTimedecimalidinstantintegermarkdownoidpositiveIntstringtimeunsignedInturiurluuidAddressAgeAnnotationAttachmentCodeableConceptCodingContactPointCountDistanceDurationHumanNameIdentifierMoneyPeriodQuantityRangeRatioReferenceSampledDataSignatureTimingContactDetailContributorDataRequirementExpressionParameterDefinitionRelatedArtifactTriggerDefinitionUsageContextDosageMeta</t>
+  </si>
+  <si>
+    <t>Value of extension</t>
+  </si>
+  <si>
+    <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](http://build.fhir.org/extensibility.html) for a list).</t>
+  </si>
+  <si>
+    <t>Extension.value[x]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 </t>
   </si>
   <si>
-    <t>Extensions are always sliced by (at least) url</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>Address Key Type</t>
-  </si>
-  <si>
-    <t>To identify the type of Address Key recorded.</t>
-  </si>
-  <si>
-    <t>Extension.extension.id</t>
-  </si>
-  <si>
-    <t>Extension.extension.extension</t>
-  </si>
-  <si>
     <t>Extension.extension.url</t>
-  </si>
-  <si>
-    <t>identifies the meaning of the extension</t>
-  </si>
-  <si>
-    <t>Source of the definition for the extension code - a logical name or a URL.</t>
-  </si>
-  <si>
-    <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
-  </si>
-  <si>
-    <t>Extension.url</t>
   </si>
   <si>
     <t>Extension.extension.value[x]</t>
@@ -246,9 +282,6 @@
 </t>
   </si>
   <si>
-    <t>A stream of bytes, base64 encoded</t>
-  </si>
-  <si>
     <t>extensible</t>
   </si>
   <si>
@@ -258,27 +291,10 @@
     <t>https://fhir.nhs.uk/R4/ValueSet/UKCore-AddressKeyType</t>
   </si>
   <si>
-    <t>Extension.value[x]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
-    <t>Value of extension</t>
-  </si>
-  <si>
-    <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](extensibility.html) for a list).</t>
-  </si>
-  <si>
     <t>https://fhir.nhs.uk/R4/StructureDefinition/Extension-UKCore-AddressKey</t>
-  </si>
-  <si>
-    <t>base64Binary
-booleancanonicalcodedatedateTimedecimalidinstantintegermarkdownoidpositiveIntstringtimeunsignedInturiurluuidAddressAgeAnnotationAttachmentCodeableConceptCodingContactPointCountDistanceDurationHumanNameIdentifierMoneyPeriodQuantityRangeRatioReferenceSampledDataSignatureTimingContactDetailContributorDataRequirementExpressionParameterDefinitionRelatedArtifactTriggerDefinitionUsageContextDosage</t>
   </si>
 </sst>
 </file>
@@ -427,7 +443,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AJ16"/>
+  <dimension ref="A1:AJ24"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -436,7 +452,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="28.2734375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="37.546875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.3828125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
@@ -681,12 +697,12 @@
         <v>43</v>
       </c>
       <c r="AJ2" t="s" s="2">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
@@ -697,25 +713,25 @@
         <v>38</v>
       </c>
       <c r="F3" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H3" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I3" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J3" t="s" s="2">
         <v>46</v>
       </c>
-      <c r="G3" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="H3" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="I3" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="J3" t="s" s="2">
+      <c r="K3" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="K3" t="s" s="2">
+      <c r="L3" t="s" s="2">
         <v>48</v>
-      </c>
-      <c r="L3" t="s" s="2">
-        <v>49</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -766,31 +782,31 @@
         <v>37</v>
       </c>
       <c r="AE3" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AF3" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG3" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH3" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI3" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AJ3" t="s" s="2">
         <v>50</v>
-      </c>
-      <c r="AF3" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AG3" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AH3" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AI3" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AJ3" t="s" s="2">
-        <v>51</v>
       </c>
     </row>
     <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
@@ -809,17 +825,15 @@
         <v>37</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="M4" t="s" s="2">
-        <v>57</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" t="s" s="2">
         <v>37</v>
@@ -856,19 +870,19 @@
         <v>37</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="AC4" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AF4" t="s" s="2">
         <v>38</v>
@@ -877,31 +891,31 @@
         <v>39</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="AI4" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" t="s" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5" t="s" s="2">
         <v>37</v>
@@ -913,17 +927,15 @@
         <v>37</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>64</v>
-      </c>
-      <c r="M5" t="s" s="2">
-        <v>57</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
         <v>37</v>
@@ -972,7 +984,7 @@
         <v>37</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AF5" t="s" s="2">
         <v>38</v>
@@ -981,18 +993,18 @@
         <v>39</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="AI5" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -1003,25 +1015,25 @@
         <v>38</v>
       </c>
       <c r="F6" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I6" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J6" t="s" s="2">
         <v>46</v>
       </c>
-      <c r="G6" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="H6" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="I6" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="J6" t="s" s="2">
+      <c r="K6" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="K6" t="s" s="2">
+      <c r="L6" t="s" s="2">
         <v>48</v>
-      </c>
-      <c r="L6" t="s" s="2">
-        <v>49</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1072,31 +1084,31 @@
         <v>37</v>
       </c>
       <c r="AE6" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AF6" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG6" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH6" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI6" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AJ6" t="s" s="2">
         <v>50</v>
-      </c>
-      <c r="AF6" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AG6" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AH6" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AI6" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AJ6" t="s" s="2">
-        <v>51</v>
       </c>
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s" s="2">
@@ -1115,16 +1127,16 @@
         <v>37</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" t="s" s="2">
@@ -1162,19 +1174,19 @@
         <v>37</v>
       </c>
       <c r="AA7" t="s" s="2">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AB7" t="s" s="2">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="AC7" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD7" t="s" s="2">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="AE7" t="s" s="2">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AF7" t="s" s="2">
         <v>38</v>
@@ -1183,13 +1195,13 @@
         <v>39</v>
       </c>
       <c r="AH7" t="s" s="2">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="AI7" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AJ7" t="s" s="2">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" hidden="true">
@@ -1202,39 +1214,37 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="G8" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H8" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I8" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J8" t="s" s="2">
         <v>46</v>
       </c>
-      <c r="F8" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="G8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="H8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="I8" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="J8" t="s" s="2">
+      <c r="K8" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="K8" t="s" s="2">
-        <v>68</v>
-      </c>
       <c r="L8" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="M8" t="s" s="2">
-        <v>70</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
         <v>37</v>
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" t="s" s="2">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="R8" t="s" s="2">
         <v>37</v>
@@ -1276,13 +1286,13 @@
         <v>37</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="AG8" t="s" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AH8" t="s" s="2">
         <v>37</v>
@@ -1291,23 +1301,23 @@
         <v>37</v>
       </c>
       <c r="AJ8" t="s" s="2">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G9" t="s" s="2">
         <v>37</v>
@@ -1319,16 +1329,16 @@
         <v>37</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
@@ -1354,64 +1364,62 @@
         <v>37</v>
       </c>
       <c r="W9" t="s" s="2">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="X9" t="s" s="2">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="Y9" t="s" s="2">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="Z9" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AA9" t="s" s="2">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="AB9" t="s" s="2">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="AC9" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD9" t="s" s="2">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AG9" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="AH9" t="s" s="2">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="B10" t="s" s="2">
-        <v>80</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G10" t="s" s="2">
         <v>37</v>
@@ -1423,16 +1431,16 @@
         <v>37</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
@@ -1482,27 +1490,27 @@
         <v>37</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="AG10" t="s" s="2">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="AH10" t="s" s="2">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>44</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
@@ -1513,7 +1521,7 @@
         <v>38</v>
       </c>
       <c r="F11" t="s" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G11" t="s" s="2">
         <v>37</v>
@@ -1525,13 +1533,13 @@
         <v>37</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1582,38 +1590,38 @@
         <v>37</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AG11" t="s" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AH11" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>51</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G12" t="s" s="2">
         <v>37</v>
@@ -1625,16 +1633,16 @@
         <v>37</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
@@ -1642,7 +1650,7 @@
       </c>
       <c r="P12" s="2"/>
       <c r="Q12" t="s" s="2">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="R12" t="s" s="2">
         <v>37</v>
@@ -1672,39 +1680,39 @@
         <v>37</v>
       </c>
       <c r="AA12" t="s" s="2">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="AB12" t="s" s="2">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="AC12" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD12" t="s" s="2">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="AG12" t="s" s="2">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="AH12" t="s" s="2">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>44</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -1712,10 +1720,10 @@
       </c>
       <c r="D13" s="2"/>
       <c r="E13" t="s" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G13" t="s" s="2">
         <v>37</v>
@@ -1727,97 +1735,97 @@
         <v>37</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="M13" t="s" s="2">
-        <v>70</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
         <v>37</v>
       </c>
       <c r="P13" s="2"/>
       <c r="Q13" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="R13" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S13" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T13" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U13" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V13" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W13" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="X13" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="Y13" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="Z13" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA13" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB13" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC13" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD13" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE13" t="s" s="2">
         <v>80</v>
       </c>
-      <c r="R13" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="S13" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="T13" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="U13" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="V13" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="W13" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="X13" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Y13" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="Z13" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AA13" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB13" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC13" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD13" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AE13" t="s" s="2">
-        <v>71</v>
-      </c>
       <c r="AF13" t="s" s="2">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="AG13" t="s" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AH13" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>44</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>88</v>
+      </c>
       <c r="C14" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F14" t="s" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G14" t="s" s="2">
         <v>37</v>
@@ -1829,17 +1837,15 @@
         <v>37</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>81</v>
+        <v>36</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="M14" t="s" s="2">
-        <v>74</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
         <v>37</v>
@@ -1888,27 +1894,27 @@
         <v>37</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AG14" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="AH14" t="s" s="2">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -1916,39 +1922,37 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="G15" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H15" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I15" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J15" t="s" s="2">
         <v>46</v>
       </c>
-      <c r="F15" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="G15" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="H15" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="I15" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="J15" t="s" s="2">
+      <c r="K15" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="K15" t="s" s="2">
-        <v>68</v>
-      </c>
       <c r="L15" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="M15" t="s" s="2">
-        <v>70</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
         <v>37</v>
       </c>
       <c r="P15" s="2"/>
       <c r="Q15" t="s" s="2">
-        <v>83</v>
+        <v>37</v>
       </c>
       <c r="R15" t="s" s="2">
         <v>37</v>
@@ -1990,13 +1994,13 @@
         <v>37</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="AG15" t="s" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AH15" t="s" s="2">
         <v>37</v>
@@ -2005,23 +2009,23 @@
         <v>37</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
         <v>38</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G16" t="s" s="2">
         <v>37</v>
@@ -2033,16 +2037,16 @@
         <v>37</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -2080,38 +2084,846 @@
         <v>37</v>
       </c>
       <c r="AA16" t="s" s="2">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="AB16" t="s" s="2">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="AC16" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD16" t="s" s="2">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="AE16" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AF16" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG16" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AH16" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI16" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AJ16" t="s" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" hidden="true">
+      <c r="A17" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F17" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="G17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J17" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="K17" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="L17" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="P17" s="2"/>
+      <c r="Q17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="R17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE17" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AF17" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG17" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AJ17" t="s" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" hidden="true">
+      <c r="A18" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F18" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="G18" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H18" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I18" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J18" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K18" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="L18" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="M18" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="N18" s="2"/>
+      <c r="O18" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="P18" s="2"/>
+      <c r="Q18" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="R18" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S18" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T18" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U18" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V18" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W18" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X18" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y18" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z18" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA18" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="AB18" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AC18" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD18" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AE18" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AF18" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG18" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AH18" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI18" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AJ18" t="s" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" hidden="true">
+      <c r="A19" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="F19" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="G19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J19" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="K19" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="L19" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="M19" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="N19" s="2"/>
+      <c r="O19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="P19" s="2"/>
+      <c r="Q19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="R19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE19" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF19" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AG19" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AJ19" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" hidden="true">
+      <c r="A20" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F20" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="G20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J20" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="K20" t="s" s="2">
         <v>78</v>
       </c>
-      <c r="AF16" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AG16" t="s" s="2">
+      <c r="L20" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="P20" s="2"/>
+      <c r="Q20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="R20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE20" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF20" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG20" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI20" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ20" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" hidden="true">
+      <c r="A21" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="F21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="G21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J21" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="K21" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="L21" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="M21" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="N21" s="2"/>
+      <c r="O21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="P21" s="2"/>
+      <c r="Q21" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="R21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE21" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AG21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AJ21" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" hidden="true">
+      <c r="A22" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F22" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="G22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J22" t="s" s="2">
         <v>46</v>
       </c>
-      <c r="AH16" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AI16" t="s" s="2">
+      <c r="K22" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="L22" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="AJ16" t="s" s="2">
-        <v>44</v>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="P22" s="2"/>
+      <c r="Q22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="R22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE22" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF22" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG22" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI22" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ22" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" hidden="true">
+      <c r="A23" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="F23" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="G23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J23" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="K23" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="L23" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="M23" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="N23" s="2"/>
+      <c r="O23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="P23" s="2"/>
+      <c r="Q23" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="R23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE23" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF23" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AG23" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AJ23" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" hidden="true">
+      <c r="A24" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F24" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="G24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J24" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="K24" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="L24" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="P24" s="2"/>
+      <c r="Q24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="R24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE24" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF24" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG24" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI24" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ24" t="s" s="2">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AJ16">
+  <autoFilter ref="A1:AJ24">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -2121,7 +2933,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI15">
+  <conditionalFormatting sqref="A2:AI23">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>